<commit_message>
Corrected Lookup xl file
</commit_message>
<xml_diff>
--- a/Ledgers/Lookup.xlsx
+++ b/Ledgers/Lookup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andre\Desktop\Golang Personal Finance\Ledgers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DE20B34-005E-4256-8536-3E9DA1989DED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E11DA9C-F196-4606-B44D-85D426FBA5B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="705" yWindow="690" windowWidth="28800" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -391,7 +391,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -423,6 +423,9 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
@@ -431,6 +434,9 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
@@ -439,6 +445,9 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>1</v>
+      </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
@@ -447,6 +456,9 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>1</v>
+      </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
@@ -455,6 +467,9 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>1</v>
+      </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
@@ -463,6 +478,9 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>1</v>
+      </c>
       <c r="B8" t="s">
         <v>9</v>
       </c>
@@ -471,6 +489,9 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>1</v>
+      </c>
       <c r="B9" t="s">
         <v>10</v>
       </c>
@@ -479,6 +500,9 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>1</v>
+      </c>
       <c r="B10" t="s">
         <v>11</v>
       </c>
@@ -487,6 +511,9 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>1</v>
+      </c>
       <c r="B11" t="s">
         <v>12</v>
       </c>

</xml_diff>